<commit_message>
Add GCM115R capacitor + correct footprint
</commit_message>
<xml_diff>
--- a/ceramic_capacitors (2).xlsx
+++ b/ceramic_capacitors (2).xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mtupi\Documents\AD22\Library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{BC69050C-A6B7-4067-B790-C08FC183D73A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FCB8DF1-1023-4E24-A6F7-D2E853BC7D00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120"/>
+    <workbookView xWindow="11475" yWindow="540" windowWidth="33570" windowHeight="19215" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ceramic_capacitors (2)" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="737" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="170">
   <si>
     <t>Description</t>
   </si>
@@ -34,417 +34,120 @@
     <t>Murata Electronics</t>
   </si>
   <si>
-    <t>CAP CER 100PF 25V C0G/NP0 01005</t>
-  </si>
-  <si>
-    <t>100 pF</t>
-  </si>
-  <si>
-    <t>±5%</t>
-  </si>
-  <si>
     <t>25V</t>
   </si>
   <si>
-    <t>C0G, NP0</t>
-  </si>
-  <si>
     <t>GRM0225C1E330JA02L</t>
   </si>
   <si>
-    <t>CAP CER 33PF 25V C0G/NP0 01005</t>
-  </si>
-  <si>
-    <t>33 pF</t>
-  </si>
-  <si>
     <t>GRM0225C1E470JA02L</t>
   </si>
   <si>
-    <t>CAP CER 47PF 25V C0G/NP0 01005</t>
-  </si>
-  <si>
-    <t>47 pF</t>
-  </si>
-  <si>
     <t>GRM0225C1E560JA02L</t>
   </si>
   <si>
-    <t>CAP CER 56PF 25V C0G/NP0 01005</t>
-  </si>
-  <si>
-    <t>56 pF</t>
-  </si>
-  <si>
     <t>GRM0225C1C100JA03L</t>
   </si>
   <si>
-    <t>CAP CER 10PF 16V C0G/NP0 01005</t>
-  </si>
-  <si>
-    <t>10 pF</t>
-  </si>
-  <si>
     <t>16V</t>
   </si>
   <si>
     <t>GRM0225C1E100JA03L</t>
   </si>
   <si>
-    <t>CAP CER 10PF 25V C0G/NP0 01005</t>
-  </si>
-  <si>
     <t>GRM0225C1E150JA03L</t>
   </si>
   <si>
-    <t>CAP CER 15PF 25V C0G/NP0 01005</t>
-  </si>
-  <si>
-    <t>15 pF</t>
-  </si>
-  <si>
     <t>GRM0225C1E220JA02L</t>
   </si>
   <si>
-    <t>CAP CER 22PF 25V C0G/NP0 01005</t>
-  </si>
-  <si>
-    <t>22 pF</t>
-  </si>
-  <si>
     <t>GRM0225C1ER30WA03L</t>
   </si>
   <si>
-    <t>CAP CER 0.3PF 25V C0G/NP0 01005</t>
-  </si>
-  <si>
-    <t>0.3 pF</t>
-  </si>
-  <si>
-    <t>±0.05pF</t>
-  </si>
-  <si>
     <t>GRM0225C1ER50WA03L</t>
   </si>
   <si>
-    <t>CAP CER 0.5PF 25V C0G/NP0 01005</t>
-  </si>
-  <si>
-    <t>0.5 pF</t>
-  </si>
-  <si>
     <t>GRM0225C1E7R0WA03L</t>
   </si>
   <si>
-    <t>CAP CER 7PF 25V C0G/NP0 01005</t>
-  </si>
-  <si>
-    <t>7 pF</t>
-  </si>
-  <si>
     <t>GRM0225C1E1R5WA03L</t>
   </si>
   <si>
-    <t>CAP CER 1.5PF 25V C0G/NP0 01005</t>
-  </si>
-  <si>
-    <t>1.5 pF</t>
-  </si>
-  <si>
     <t>GRM0225C1E3R9WA03L</t>
   </si>
   <si>
-    <t>CAP CER 3.9PF 25V C0G/NP0 01005</t>
-  </si>
-  <si>
-    <t>3.9 pF</t>
-  </si>
-  <si>
     <t>GRM0225CYA101JA02L</t>
   </si>
   <si>
-    <t>CAP CER 100PF 35V C0G/NP0 01005</t>
-  </si>
-  <si>
-    <t>35V</t>
-  </si>
-  <si>
     <t>GRM0225C1HR80WA03L</t>
   </si>
   <si>
-    <t>CAP CER 0.8PF 50V C0G/NP0 01005</t>
-  </si>
-  <si>
-    <t>0.8 pF</t>
-  </si>
-  <si>
     <t>50V</t>
   </si>
   <si>
     <t>GRM0225C1E221JA02L</t>
   </si>
   <si>
-    <t>CAP CER 220PF 25V C0G/NP0 01005</t>
-  </si>
-  <si>
     <t>220 pF</t>
   </si>
   <si>
     <t>GRM0225C1ER20WA03L</t>
   </si>
   <si>
-    <t>CAP CER 0.2PF 25V C0G/NP0 01005</t>
-  </si>
-  <si>
-    <t>0.2 pF</t>
-  </si>
-  <si>
     <t>GRM0225C1H150JA03L</t>
   </si>
   <si>
-    <t>CAP CER 15PF 50V C0G/NP0 01005</t>
-  </si>
-  <si>
     <t>GRM0225C1C121JA02L</t>
   </si>
   <si>
-    <t>CAP CER 120PF 16V C0G/NP0 01005</t>
-  </si>
-  <si>
-    <t>120 pF</t>
-  </si>
-  <si>
     <t>GRM0225C1H100JA03L</t>
   </si>
   <si>
-    <t>CAP CER 10PF 50V C0G/NP0 01005</t>
-  </si>
-  <si>
     <t>GRM0225C1H120JA03L</t>
   </si>
   <si>
-    <t>CAP CER 12PF 50V C0G/NP0 01005</t>
-  </si>
-  <si>
-    <t>12 pF</t>
-  </si>
-  <si>
     <t>GRM0225C1H820JA02L</t>
   </si>
   <si>
-    <t>CAP CER 82PF 50V C0G/NP0 01005</t>
-  </si>
-  <si>
-    <t>82 pF</t>
-  </si>
-  <si>
     <t>GRM0225C1C120JA03L</t>
   </si>
   <si>
-    <t>CAP CER 12PF 16V C0G/NP0 01005</t>
-  </si>
-  <si>
     <t>GRM0225C1C270JA02L</t>
   </si>
   <si>
-    <t>CAP CER 27PF 16V C0G/NP0 01005</t>
-  </si>
-  <si>
-    <t>27 pF</t>
-  </si>
-  <si>
     <t>GRM0225C1E120JA03L</t>
   </si>
   <si>
-    <t>CAP CER 12PF 25V C0G/NP0 01005</t>
-  </si>
-  <si>
     <t>GRM0225C1H101JA02L</t>
   </si>
   <si>
-    <t>CAP CER 100PF 50V C0G/NP0 01005</t>
-  </si>
-  <si>
     <t>GRM0225C1H470JA02L</t>
   </si>
   <si>
-    <t>CAP CER 47PF 50V C0G/NP0 01005</t>
-  </si>
-  <si>
     <t>GRM0225C1H330JA02L</t>
   </si>
   <si>
-    <t>CAP CER 33PF 50V C0G/NP0 01005</t>
-  </si>
-  <si>
     <t>GRM0225C1E270JA02L</t>
   </si>
   <si>
-    <t>CAP CER 27PF 25V C0G/NP0 01005</t>
-  </si>
-  <si>
     <t>GRM0225C1ER80WA03L</t>
   </si>
   <si>
-    <t>CAP CER 0.8PF 25V C0G/NP0 01005</t>
-  </si>
-  <si>
     <t>GRM0225C1E820JA02L</t>
   </si>
   <si>
-    <t>CAP CER 82PF 25V C0G/NP0 01005</t>
-  </si>
-  <si>
     <t>GRM0225C1H220JA02L</t>
   </si>
   <si>
-    <t>CAP CER 22PF 50V C0G/NP0 01005</t>
-  </si>
-  <si>
     <t>GRM0225C1E180JA02L</t>
   </si>
   <si>
-    <t>CAP CER 18PF 25V C0G/NP0 01005</t>
-  </si>
-  <si>
-    <t>18 pF</t>
-  </si>
-  <si>
     <t>GRM0225C1ER40WA03L</t>
   </si>
   <si>
-    <t>CAP CER 0.4PF 25V C0G/NP0 01005</t>
-  </si>
-  <si>
-    <t>0.4 pF</t>
-  </si>
-  <si>
     <t>GRM0225C1E8R0WA03L</t>
   </si>
   <si>
-    <t>CAP CER 8PF 25V C0G/NP0 01005</t>
-  </si>
-  <si>
-    <t>8 pF</t>
-  </si>
-  <si>
-    <t>GRM0225C1E5R0WA03L</t>
-  </si>
-  <si>
-    <t>CAP CER 5PF 25V C0G/NP0 01005</t>
-  </si>
-  <si>
-    <t>5 pF</t>
-  </si>
-  <si>
-    <t>GRM0225C1E4R7WA03L</t>
-  </si>
-  <si>
-    <t>CAP CER 4.7PF 25V C0G/NP0 01005</t>
-  </si>
-  <si>
-    <t>4.7 pF</t>
-  </si>
-  <si>
-    <t>GRM0225C1E2R0WA03L</t>
-  </si>
-  <si>
-    <t>CAP CER 2PF 25V C0G/NP0 01005</t>
-  </si>
-  <si>
-    <t>2 pF</t>
-  </si>
-  <si>
-    <t>GRM0225C1E4R1WA03L</t>
-  </si>
-  <si>
-    <t>CAP CER 4.1PF 25V C0G/NP0 01005</t>
-  </si>
-  <si>
-    <t>4.1 pF</t>
-  </si>
-  <si>
-    <t>GRM0225C1E1R2WA03L</t>
-  </si>
-  <si>
-    <t>CAP CER 1.2PF 25V C0G/NP0 01005</t>
-  </si>
-  <si>
-    <t>1.2 pF</t>
-  </si>
-  <si>
-    <t>GRM0225C1E5R6WA03L</t>
-  </si>
-  <si>
-    <t>CAP CER 5.6PF 25V C0G/NP0 01005</t>
-  </si>
-  <si>
-    <t>5.6 pF</t>
-  </si>
-  <si>
-    <t>GRM0225C1E1R9WA03L</t>
-  </si>
-  <si>
-    <t>CAP CER 1.9PF 25V C0G/NP0 01005</t>
-  </si>
-  <si>
-    <t>1.9 pF</t>
-  </si>
-  <si>
-    <t>GRM0225C1E1R0WA03L</t>
-  </si>
-  <si>
-    <t>CAP CER 1PF 25V C0G/NP0 01005</t>
-  </si>
-  <si>
-    <t>1 pF</t>
-  </si>
-  <si>
-    <t>GRM0225C1E1R8WA03L</t>
-  </si>
-  <si>
-    <t>CAP CER 1.8PF 25V C0G/NP0 01005</t>
-  </si>
-  <si>
-    <t>1.8 pF</t>
-  </si>
-  <si>
-    <t>GRM0225C1E5R4WA03L</t>
-  </si>
-  <si>
-    <t>CAP CER 5.4PF 25V C0G/NP0 01005</t>
-  </si>
-  <si>
-    <t>5.4 pF</t>
-  </si>
-  <si>
-    <t>GRM0225C1E9R0WA03L</t>
-  </si>
-  <si>
-    <t>CAP CER 9PF 25V C0G/NP0 01005</t>
-  </si>
-  <si>
-    <t>9 pF</t>
-  </si>
-  <si>
-    <t>GRM0225C1E1R7WA03L</t>
-  </si>
-  <si>
-    <t>CAP CER 1.7PF 25V C0G/NP0 01005</t>
-  </si>
-  <si>
-    <t>1.7 pF</t>
-  </si>
-  <si>
-    <t>GRM0225C1E3R4WA03L</t>
-  </si>
-  <si>
-    <t>CAP CER 3.4PF 25V C0G/NP0 01005</t>
-  </si>
-  <si>
-    <t>3.4 pF</t>
-  </si>
-  <si>
     <t>Capacitance Tolerance</t>
   </si>
   <si>
@@ -496,9 +199,6 @@
     <t>CAP_2pin</t>
   </si>
   <si>
-    <t>CAP0603</t>
-  </si>
-  <si>
     <t>Symbols\Capacitor.SchLib</t>
   </si>
   <si>
@@ -509,12 +209,333 @@
   </si>
   <si>
     <t>0402</t>
+  </si>
+  <si>
+    <t>GCM155R71H123KA55D</t>
+  </si>
+  <si>
+    <t>GCM155R71H153KA55D</t>
+  </si>
+  <si>
+    <t>GCM155R71H183KA55D</t>
+  </si>
+  <si>
+    <t>GCM155R71H223KA55D</t>
+  </si>
+  <si>
+    <t>GCM155R71E273KA55D</t>
+  </si>
+  <si>
+    <t>GCM155R71H333KE02D</t>
+  </si>
+  <si>
+    <t>GCM155R71E393KA55D</t>
+  </si>
+  <si>
+    <t>GCM155R71H473KE02D</t>
+  </si>
+  <si>
+    <t>GCM155R71C563KA55D</t>
+  </si>
+  <si>
+    <t>GCM155R71H683KE02J</t>
+  </si>
+  <si>
+    <t>GCM155R71C823KA55D</t>
+  </si>
+  <si>
+    <t>GCM155R71H104KE02J</t>
+  </si>
+  <si>
+    <t>GCM155R71C154KE02D</t>
+  </si>
+  <si>
+    <t>GCM155R71C224KE02D</t>
+  </si>
+  <si>
+    <t>GCM155R71H102KA37D</t>
+  </si>
+  <si>
+    <t>GCM155R71H103KA55D</t>
+  </si>
+  <si>
+    <t>GCM155R71H122KA37D</t>
+  </si>
+  <si>
+    <t>GCM155R71H152KA37D</t>
+  </si>
+  <si>
+    <t>GCM155R71H182KA37D</t>
+  </si>
+  <si>
+    <t>GCM155R71H221KA37D</t>
+  </si>
+  <si>
+    <t>GCM155R71H222KA37J</t>
+  </si>
+  <si>
+    <t>GCM155R71H271KA37J</t>
+  </si>
+  <si>
+    <t>GCM155R71H272KA37D</t>
+  </si>
+  <si>
+    <t>GCM155R71H331KA37D</t>
+  </si>
+  <si>
+    <t>GCM155R71H332KA37J</t>
+  </si>
+  <si>
+    <t>GCM155R71H391KA37D</t>
+  </si>
+  <si>
+    <t>GCM155R71H392KA37D</t>
+  </si>
+  <si>
+    <t>GCM155R71H471KA37D</t>
+  </si>
+  <si>
+    <t>GCM155R71H472KA37J</t>
+  </si>
+  <si>
+    <t>GCM155R71H561KA37D</t>
+  </si>
+  <si>
+    <t>GCM155R71H562KA55J</t>
+  </si>
+  <si>
+    <t>GCM155R71H681KA37D</t>
+  </si>
+  <si>
+    <t>GCM155R71H682KA55D</t>
+  </si>
+  <si>
+    <t>GCM155R71H821KA37D</t>
+  </si>
+  <si>
+    <t>GCM155R71H822KA55D</t>
+  </si>
+  <si>
+    <t>±10%</t>
+  </si>
+  <si>
+    <t>12 nF</t>
+  </si>
+  <si>
+    <t>15 nF</t>
+  </si>
+  <si>
+    <t>18 nF</t>
+  </si>
+  <si>
+    <t>22 nF</t>
+  </si>
+  <si>
+    <t>27 nF</t>
+  </si>
+  <si>
+    <t>33 nF</t>
+  </si>
+  <si>
+    <t>39 nF</t>
+  </si>
+  <si>
+    <t>47 nF</t>
+  </si>
+  <si>
+    <t>56 nF</t>
+  </si>
+  <si>
+    <t>68 nF</t>
+  </si>
+  <si>
+    <t>82 nF</t>
+  </si>
+  <si>
+    <t>100 nF</t>
+  </si>
+  <si>
+    <t>150 nF</t>
+  </si>
+  <si>
+    <t>200 nF</t>
+  </si>
+  <si>
+    <t>1 nF</t>
+  </si>
+  <si>
+    <t>10 nF</t>
+  </si>
+  <si>
+    <t>1.2 nF</t>
+  </si>
+  <si>
+    <t>1.5 nF</t>
+  </si>
+  <si>
+    <t>1.8 nF</t>
+  </si>
+  <si>
+    <t>2.2 nF</t>
+  </si>
+  <si>
+    <t>270 pF</t>
+  </si>
+  <si>
+    <t>2.7 nF</t>
+  </si>
+  <si>
+    <t>330 pF</t>
+  </si>
+  <si>
+    <t>3.3 nF</t>
+  </si>
+  <si>
+    <t>390 pF</t>
+  </si>
+  <si>
+    <t>3.9 nF</t>
+  </si>
+  <si>
+    <t>470 pF</t>
+  </si>
+  <si>
+    <t>4.7 nF</t>
+  </si>
+  <si>
+    <t>560 pF</t>
+  </si>
+  <si>
+    <t>5.6 nF</t>
+  </si>
+  <si>
+    <t>680 pF</t>
+  </si>
+  <si>
+    <t>6.8 nF</t>
+  </si>
+  <si>
+    <t>820 pF</t>
+  </si>
+  <si>
+    <t>8.2 nF</t>
+  </si>
+  <si>
+    <t>CAP0402</t>
+  </si>
+  <si>
+    <t>CAP CER 0.012UF 50V X7R 0402</t>
+  </si>
+  <si>
+    <t>CAP CER 0.015UF 50V X7R 0402</t>
+  </si>
+  <si>
+    <t>CAP CER 0.018UF 50V X7R 0402</t>
+  </si>
+  <si>
+    <t>CAP CER 0.022UF 50V X7R 0402</t>
+  </si>
+  <si>
+    <t>CAP CER 0.027UF 25V X7R 0402</t>
+  </si>
+  <si>
+    <t>CAP CER 0.033UF 50V X7R 0402</t>
+  </si>
+  <si>
+    <t>CAP CER 0.039UF 25V X7R 0402</t>
+  </si>
+  <si>
+    <t>CAP CER 0.047UF 50V X7R 0402</t>
+  </si>
+  <si>
+    <t>CAP CER 0.056UF 16V X7R 0402</t>
+  </si>
+  <si>
+    <t>CAP CER 0.068UF 50V X7R 0402</t>
+  </si>
+  <si>
+    <t>CAP CER 0.082UF 16V X7R 0402</t>
+  </si>
+  <si>
+    <t>CAP CER 0.1UF 50V X7R 0402</t>
+  </si>
+  <si>
+    <t>CAP CER 0.15UF 16V X7R 0402</t>
+  </si>
+  <si>
+    <t>CAP CER 0.22UF 16V X7R 0402</t>
+  </si>
+  <si>
+    <t>CAP CER 1000PF 50V X7R 0402</t>
+  </si>
+  <si>
+    <t>CAP CER 10000PF 50V X7R 0402</t>
+  </si>
+  <si>
+    <t>CAP CER 1200PF 50V X7R 0402</t>
+  </si>
+  <si>
+    <t>CAP CER 1500PF 50V X7R 0402</t>
+  </si>
+  <si>
+    <t>CAP CER 1800PF 50V X7R 0402</t>
+  </si>
+  <si>
+    <t>CAP CER 220PF 50V X7R 0402</t>
+  </si>
+  <si>
+    <t>CAP CER 2200PF 50V X7R 0402</t>
+  </si>
+  <si>
+    <t>CAP CER 270PF 50V X7R 0402</t>
+  </si>
+  <si>
+    <t>CAP CER 2700PF 50V X7R 0402</t>
+  </si>
+  <si>
+    <t>CAP CER 330PF 50V X7R 0402</t>
+  </si>
+  <si>
+    <t>CAP CER 3300PF 50V X7R 0402</t>
+  </si>
+  <si>
+    <t>CAP CER 390PF 50V X7R 0402</t>
+  </si>
+  <si>
+    <t>CAP CER 3900PF 50V X7R 0402</t>
+  </si>
+  <si>
+    <t>CAP CER 470PF 50V X7R 0402</t>
+  </si>
+  <si>
+    <t>CAP CER 4700PF 50V X7R 0402</t>
+  </si>
+  <si>
+    <t>CAP CER 560PF 50V X7R 0402</t>
+  </si>
+  <si>
+    <t>CAP CER 5600PF 50V X7R 0402</t>
+  </si>
+  <si>
+    <t>CAP CER 680PF 50V X7R 0402</t>
+  </si>
+  <si>
+    <t>CAP CER 6800PF 50V X7R 0402</t>
+  </si>
+  <si>
+    <t>CAP CER 820PF 50V X7R 0402</t>
+  </si>
+  <si>
+    <t>CAP CER 8200PF 50V X7R 0402</t>
+  </si>
+  <si>
+    <t>X7R</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1050,10 +1071,10 @@
     <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="42" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="42" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1095,7 +1116,7 @@
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal_ceramic_capacitors (2)" xfId="42"/>
+    <cellStyle name="Normal_ceramic_capacitors (2)" xfId="42" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
@@ -1411,11 +1432,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T20" sqref="T20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2:O36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1440,1611 +1461,1611 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>141</v>
+        <v>42</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>142</v>
+        <v>43</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>143</v>
+        <v>44</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>144</v>
+        <v>45</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>145</v>
+        <v>46</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>146</v>
+        <v>47</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>147</v>
+        <v>48</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>148</v>
+        <v>49</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>149</v>
+        <v>50</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>150</v>
+        <v>51</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>151</v>
+        <v>52</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>152</v>
+        <v>53</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>153</v>
+        <v>54</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>154</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>162</v>
+        <v>62</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>155</v>
+        <v>56</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>156</v>
+        <v>57</v>
       </c>
       <c r="G2" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="H2" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="I2" t="s">
         <v>2</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>157</v>
+        <v>58</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>159</v>
+        <v>59</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>160</v>
+        <v>60</v>
       </c>
       <c r="N2" t="s">
-        <v>4</v>
+        <v>134</v>
       </c>
       <c r="O2" t="s">
-        <v>8</v>
+        <v>169</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>161</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>98</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>64</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>162</v>
+        <v>62</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>155</v>
+        <v>56</v>
       </c>
       <c r="G3" t="s">
-        <v>11</v>
+        <v>100</v>
       </c>
       <c r="H3" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="I3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>157</v>
+        <v>58</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>159</v>
+        <v>59</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>160</v>
+        <v>60</v>
       </c>
       <c r="N3" t="s">
-        <v>10</v>
+        <v>135</v>
       </c>
       <c r="O3" t="s">
-        <v>8</v>
+        <v>169</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>161</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" t="s">
+        <v>101</v>
+      </c>
+      <c r="H4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="G4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I4" t="s">
-        <v>12</v>
-      </c>
       <c r="J4" s="2" t="s">
-        <v>157</v>
+        <v>58</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>159</v>
+        <v>59</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>160</v>
+        <v>60</v>
       </c>
       <c r="N4" t="s">
-        <v>13</v>
+        <v>136</v>
       </c>
       <c r="O4" t="s">
-        <v>8</v>
+        <v>169</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>161</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>98</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>66</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>162</v>
+        <v>62</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>155</v>
+        <v>56</v>
       </c>
       <c r="G5" t="s">
-        <v>17</v>
+        <v>102</v>
       </c>
       <c r="H5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" t="s">
         <v>7</v>
       </c>
-      <c r="I5" t="s">
-        <v>15</v>
-      </c>
       <c r="J5" s="2" t="s">
-        <v>157</v>
+        <v>58</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>159</v>
+        <v>59</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>160</v>
+        <v>60</v>
       </c>
       <c r="N5" t="s">
-        <v>16</v>
+        <v>137</v>
       </c>
       <c r="O5" t="s">
-        <v>8</v>
+        <v>169</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>161</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>98</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="C6" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>162</v>
+        <v>62</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>155</v>
+        <v>56</v>
       </c>
       <c r="G6" t="s">
-        <v>20</v>
+        <v>103</v>
       </c>
       <c r="H6" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="I6" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>157</v>
+        <v>58</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>159</v>
+        <v>59</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>160</v>
+        <v>60</v>
       </c>
       <c r="N6" t="s">
-        <v>19</v>
+        <v>138</v>
       </c>
       <c r="O6" t="s">
-        <v>8</v>
+        <v>169</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>161</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>98</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="C7" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>162</v>
+        <v>62</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>155</v>
+        <v>56</v>
       </c>
       <c r="G7" t="s">
+        <v>104</v>
+      </c>
+      <c r="H7" t="s">
         <v>20</v>
       </c>
-      <c r="H7" t="s">
-        <v>7</v>
-      </c>
       <c r="I7" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>157</v>
+        <v>58</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>159</v>
+        <v>59</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>160</v>
+        <v>60</v>
       </c>
       <c r="N7" t="s">
-        <v>23</v>
+        <v>139</v>
       </c>
       <c r="O7" t="s">
-        <v>8</v>
+        <v>169</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>161</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>98</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>69</v>
       </c>
       <c r="C8" t="s">
         <v>3</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>162</v>
+        <v>62</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>155</v>
+        <v>56</v>
       </c>
       <c r="G8" t="s">
-        <v>26</v>
+        <v>105</v>
       </c>
       <c r="H8" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I8" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>157</v>
+        <v>58</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>159</v>
+        <v>59</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>160</v>
+        <v>60</v>
       </c>
       <c r="N8" t="s">
-        <v>25</v>
+        <v>140</v>
       </c>
       <c r="O8" t="s">
-        <v>8</v>
+        <v>169</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>161</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>98</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="C9" t="s">
         <v>3</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>162</v>
+        <v>62</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>155</v>
+        <v>56</v>
       </c>
       <c r="G9" t="s">
-        <v>29</v>
+        <v>106</v>
       </c>
       <c r="H9" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="I9" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>157</v>
+        <v>58</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>159</v>
+        <v>59</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>160</v>
+        <v>60</v>
       </c>
       <c r="N9" t="s">
-        <v>28</v>
+        <v>141</v>
       </c>
       <c r="O9" t="s">
-        <v>8</v>
+        <v>169</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>161</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>98</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>71</v>
       </c>
       <c r="C10" t="s">
         <v>3</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>162</v>
+        <v>62</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>155</v>
+        <v>56</v>
       </c>
       <c r="G10" t="s">
-        <v>32</v>
+        <v>107</v>
       </c>
       <c r="H10" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="I10" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>157</v>
+        <v>58</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>159</v>
+        <v>59</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>160</v>
+        <v>60</v>
       </c>
       <c r="N10" t="s">
-        <v>31</v>
+        <v>142</v>
       </c>
       <c r="O10" t="s">
-        <v>8</v>
+        <v>169</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>161</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>98</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="C11" t="s">
         <v>3</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>162</v>
+        <v>62</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>155</v>
+        <v>56</v>
       </c>
       <c r="G11" t="s">
-        <v>36</v>
+        <v>108</v>
       </c>
       <c r="H11" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="I11" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>157</v>
+        <v>58</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>159</v>
+        <v>59</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>160</v>
+        <v>60</v>
       </c>
       <c r="N11" t="s">
-        <v>35</v>
+        <v>143</v>
       </c>
       <c r="O11" t="s">
-        <v>8</v>
+        <v>169</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>161</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>98</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>73</v>
       </c>
       <c r="C12" t="s">
         <v>3</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>162</v>
+        <v>62</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>155</v>
+        <v>56</v>
       </c>
       <c r="G12" t="s">
-        <v>39</v>
+        <v>109</v>
       </c>
       <c r="H12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="I12" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>157</v>
+        <v>58</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>159</v>
+        <v>59</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>160</v>
+        <v>60</v>
       </c>
       <c r="N12" t="s">
-        <v>38</v>
+        <v>144</v>
       </c>
       <c r="O12" t="s">
-        <v>8</v>
+        <v>169</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>161</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>98</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>74</v>
       </c>
       <c r="C13" t="s">
         <v>3</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>162</v>
+        <v>62</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>155</v>
+        <v>56</v>
       </c>
       <c r="G13" t="s">
-        <v>42</v>
+        <v>110</v>
       </c>
       <c r="H13" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="I13" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>157</v>
+        <v>58</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>159</v>
+        <v>59</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>160</v>
+        <v>60</v>
       </c>
       <c r="N13" t="s">
-        <v>41</v>
+        <v>145</v>
       </c>
       <c r="O13" t="s">
-        <v>8</v>
+        <v>169</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>161</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>98</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>75</v>
       </c>
       <c r="C14" t="s">
         <v>3</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>162</v>
+        <v>62</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>155</v>
+        <v>56</v>
       </c>
       <c r="G14" t="s">
-        <v>45</v>
+        <v>111</v>
       </c>
       <c r="H14" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="I14" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>157</v>
+        <v>58</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>159</v>
+        <v>59</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>160</v>
+        <v>60</v>
       </c>
       <c r="N14" t="s">
-        <v>44</v>
+        <v>146</v>
       </c>
       <c r="O14" t="s">
-        <v>8</v>
+        <v>169</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>161</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>6</v>
+        <v>98</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>76</v>
       </c>
       <c r="C15" t="s">
         <v>3</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>162</v>
+        <v>62</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>155</v>
+        <v>56</v>
       </c>
       <c r="G15" t="s">
-        <v>5</v>
+        <v>112</v>
       </c>
       <c r="H15" t="s">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="I15" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>157</v>
+        <v>58</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>159</v>
+        <v>59</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>160</v>
+        <v>60</v>
       </c>
       <c r="N15" t="s">
-        <v>47</v>
+        <v>147</v>
       </c>
       <c r="O15" t="s">
-        <v>8</v>
+        <v>169</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>161</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>33</v>
+        <v>98</v>
       </c>
       <c r="B16" t="s">
-        <v>49</v>
+        <v>77</v>
       </c>
       <c r="C16" t="s">
         <v>3</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>162</v>
+        <v>62</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>155</v>
+        <v>56</v>
       </c>
       <c r="G16" t="s">
-        <v>51</v>
+        <v>113</v>
       </c>
       <c r="H16" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="I16" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>157</v>
+        <v>58</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>159</v>
+        <v>59</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>160</v>
+        <v>60</v>
       </c>
       <c r="N16" t="s">
-        <v>50</v>
+        <v>148</v>
       </c>
       <c r="O16" t="s">
-        <v>8</v>
+        <v>169</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>161</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>6</v>
+        <v>98</v>
       </c>
       <c r="B17" t="s">
-        <v>53</v>
+        <v>78</v>
       </c>
       <c r="C17" t="s">
         <v>3</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>162</v>
+        <v>62</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>155</v>
+        <v>56</v>
       </c>
       <c r="G17" t="s">
-        <v>55</v>
+        <v>114</v>
       </c>
       <c r="H17" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="I17" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>157</v>
+        <v>58</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>159</v>
+        <v>59</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>160</v>
+        <v>60</v>
       </c>
       <c r="N17" t="s">
-        <v>54</v>
+        <v>149</v>
       </c>
       <c r="O17" t="s">
-        <v>8</v>
+        <v>169</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>161</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>33</v>
+        <v>98</v>
       </c>
       <c r="B18" t="s">
-        <v>56</v>
+        <v>79</v>
       </c>
       <c r="C18" t="s">
         <v>3</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>162</v>
+        <v>62</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>155</v>
+        <v>56</v>
       </c>
       <c r="G18" t="s">
-        <v>58</v>
+        <v>115</v>
       </c>
       <c r="H18" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="I18" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>157</v>
+        <v>58</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>159</v>
+        <v>59</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>160</v>
+        <v>60</v>
       </c>
       <c r="N18" t="s">
-        <v>57</v>
+        <v>150</v>
       </c>
       <c r="O18" t="s">
-        <v>8</v>
+        <v>169</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>161</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>6</v>
+        <v>98</v>
       </c>
       <c r="B19" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="C19" t="s">
         <v>3</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>162</v>
+        <v>62</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>155</v>
+        <v>56</v>
       </c>
       <c r="G19" t="s">
-        <v>26</v>
+        <v>116</v>
       </c>
       <c r="H19" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="I19" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>157</v>
+        <v>58</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>159</v>
+        <v>59</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>160</v>
+        <v>60</v>
       </c>
       <c r="N19" t="s">
-        <v>60</v>
+        <v>151</v>
       </c>
       <c r="O19" t="s">
-        <v>8</v>
+        <v>169</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>161</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>6</v>
+        <v>98</v>
       </c>
       <c r="B20" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="C20" t="s">
         <v>3</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>162</v>
+        <v>62</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>155</v>
+        <v>56</v>
       </c>
       <c r="G20" t="s">
-        <v>63</v>
+        <v>117</v>
       </c>
       <c r="H20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I20" t="s">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>157</v>
+        <v>58</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>159</v>
+        <v>59</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>160</v>
+        <v>60</v>
       </c>
       <c r="N20" t="s">
-        <v>62</v>
+        <v>152</v>
       </c>
       <c r="O20" t="s">
-        <v>8</v>
+        <v>169</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>161</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>6</v>
+        <v>98</v>
       </c>
       <c r="B21" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="C21" t="s">
         <v>3</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>162</v>
+        <v>62</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>155</v>
+        <v>56</v>
       </c>
       <c r="G21" t="s">
+        <v>22</v>
+      </c>
+      <c r="H21" t="s">
         <v>20</v>
       </c>
-      <c r="H21" t="s">
-        <v>52</v>
-      </c>
       <c r="I21" t="s">
-        <v>64</v>
+        <v>26</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>157</v>
+        <v>58</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>159</v>
+        <v>59</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>160</v>
+        <v>60</v>
       </c>
       <c r="N21" t="s">
-        <v>65</v>
+        <v>153</v>
       </c>
       <c r="O21" t="s">
-        <v>8</v>
+        <v>169</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>161</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>6</v>
+        <v>98</v>
       </c>
       <c r="B22" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="C22" t="s">
         <v>3</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>162</v>
+        <v>62</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>155</v>
+        <v>56</v>
       </c>
       <c r="G22" t="s">
-        <v>68</v>
+        <v>118</v>
       </c>
       <c r="H22" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="I22" t="s">
-        <v>66</v>
+        <v>27</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>157</v>
+        <v>58</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>159</v>
+        <v>59</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>160</v>
+        <v>60</v>
       </c>
       <c r="N22" t="s">
-        <v>67</v>
+        <v>154</v>
       </c>
       <c r="O22" t="s">
-        <v>8</v>
+        <v>169</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>161</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>6</v>
+        <v>98</v>
       </c>
       <c r="B23" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="C23" t="s">
         <v>3</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>162</v>
+        <v>62</v>
       </c>
       <c r="E23" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G23" t="s">
+        <v>119</v>
+      </c>
+      <c r="H23" t="s">
+        <v>20</v>
+      </c>
+      <c r="I23" t="s">
+        <v>28</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="N23" t="s">
         <v>155</v>
       </c>
-      <c r="G23" t="s">
-        <v>71</v>
-      </c>
-      <c r="H23" t="s">
-        <v>52</v>
-      </c>
-      <c r="I23" t="s">
-        <v>69</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="K23" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="L23" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="M23" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="N23" t="s">
-        <v>70</v>
-      </c>
       <c r="O23" t="s">
-        <v>8</v>
+        <v>169</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>161</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>6</v>
+        <v>98</v>
       </c>
       <c r="B24" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="C24" t="s">
         <v>3</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>162</v>
+        <v>62</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>155</v>
+        <v>56</v>
       </c>
       <c r="G24" t="s">
-        <v>68</v>
+        <v>120</v>
       </c>
       <c r="H24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I24" t="s">
-        <v>72</v>
+        <v>29</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>157</v>
+        <v>58</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>159</v>
+        <v>59</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>160</v>
+        <v>60</v>
       </c>
       <c r="N24" t="s">
-        <v>73</v>
+        <v>156</v>
       </c>
       <c r="O24" t="s">
-        <v>8</v>
+        <v>169</v>
       </c>
       <c r="P24" s="2" t="s">
-        <v>161</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>6</v>
+        <v>98</v>
       </c>
       <c r="B25" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="C25" t="s">
         <v>3</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>162</v>
+        <v>62</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>155</v>
+        <v>56</v>
       </c>
       <c r="G25" t="s">
-        <v>76</v>
+        <v>121</v>
       </c>
       <c r="H25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I25" t="s">
-        <v>74</v>
+        <v>30</v>
       </c>
       <c r="J25" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M25" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="N25" t="s">
         <v>157</v>
       </c>
-      <c r="K25" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="L25" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="M25" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="N25" t="s">
-        <v>75</v>
-      </c>
       <c r="O25" t="s">
-        <v>8</v>
+        <v>169</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>161</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>6</v>
+        <v>98</v>
       </c>
       <c r="B26" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="C26" t="s">
         <v>3</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>162</v>
+        <v>62</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>155</v>
+        <v>56</v>
       </c>
       <c r="G26" t="s">
-        <v>68</v>
+        <v>122</v>
       </c>
       <c r="H26" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="I26" t="s">
-        <v>77</v>
+        <v>31</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>157</v>
+        <v>58</v>
       </c>
       <c r="K26" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="N26" t="s">
         <v>158</v>
       </c>
-      <c r="L26" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="M26" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="N26" t="s">
-        <v>78</v>
-      </c>
       <c r="O26" t="s">
-        <v>8</v>
+        <v>169</v>
       </c>
       <c r="P26" s="2" t="s">
-        <v>161</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>6</v>
+        <v>98</v>
       </c>
       <c r="B27" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="C27" t="s">
         <v>3</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>162</v>
+        <v>62</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>155</v>
+        <v>56</v>
       </c>
       <c r="G27" t="s">
-        <v>5</v>
+        <v>123</v>
       </c>
       <c r="H27" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="I27" t="s">
-        <v>79</v>
+        <v>32</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>157</v>
+        <v>58</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="L27" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="N27" t="s">
         <v>159</v>
       </c>
-      <c r="M27" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="N27" t="s">
-        <v>80</v>
-      </c>
       <c r="O27" t="s">
-        <v>8</v>
+        <v>169</v>
       </c>
       <c r="P27" s="2" t="s">
-        <v>161</v>
+        <v>61</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>6</v>
+        <v>98</v>
       </c>
       <c r="B28" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="C28" t="s">
         <v>3</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>162</v>
+        <v>62</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>155</v>
+        <v>56</v>
       </c>
       <c r="G28" t="s">
-        <v>14</v>
+        <v>124</v>
       </c>
       <c r="H28" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="I28" t="s">
-        <v>81</v>
+        <v>33</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>157</v>
+        <v>58</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>159</v>
+        <v>59</v>
       </c>
       <c r="M28" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="N28" t="s">
         <v>160</v>
       </c>
-      <c r="N28" t="s">
-        <v>82</v>
-      </c>
       <c r="O28" t="s">
-        <v>8</v>
+        <v>169</v>
       </c>
       <c r="P28" s="2" t="s">
-        <v>161</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>6</v>
+        <v>98</v>
       </c>
       <c r="B29" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="C29" t="s">
         <v>3</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>162</v>
+        <v>62</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>155</v>
+        <v>56</v>
       </c>
       <c r="G29" t="s">
-        <v>11</v>
+        <v>125</v>
       </c>
       <c r="H29" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="I29" t="s">
-        <v>83</v>
+        <v>34</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>157</v>
+        <v>58</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>159</v>
+        <v>59</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>160</v>
+        <v>60</v>
       </c>
       <c r="N29" t="s">
-        <v>84</v>
+        <v>161</v>
       </c>
       <c r="O29" t="s">
-        <v>8</v>
+        <v>169</v>
       </c>
       <c r="P29" s="2" t="s">
-        <v>161</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>6</v>
+        <v>98</v>
       </c>
       <c r="B30" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="C30" t="s">
         <v>3</v>
       </c>
       <c r="D30" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G30" t="s">
+        <v>126</v>
+      </c>
+      <c r="H30" t="s">
+        <v>20</v>
+      </c>
+      <c r="I30" t="s">
+        <v>35</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="L30" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="M30" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="N30" t="s">
         <v>162</v>
       </c>
-      <c r="E30" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="G30" t="s">
-        <v>76</v>
-      </c>
-      <c r="H30" t="s">
-        <v>7</v>
-      </c>
-      <c r="I30" t="s">
-        <v>85</v>
-      </c>
-      <c r="J30" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="K30" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="L30" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="M30" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="N30" t="s">
-        <v>86</v>
-      </c>
       <c r="O30" t="s">
-        <v>8</v>
+        <v>169</v>
       </c>
       <c r="P30" s="2" t="s">
-        <v>161</v>
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>33</v>
+        <v>98</v>
       </c>
       <c r="B31" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C31" t="s">
         <v>3</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>162</v>
+        <v>62</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>155</v>
+        <v>56</v>
       </c>
       <c r="G31" t="s">
-        <v>51</v>
+        <v>127</v>
       </c>
       <c r="H31" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="I31" t="s">
-        <v>87</v>
+        <v>36</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>157</v>
+        <v>58</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>159</v>
+        <v>59</v>
       </c>
       <c r="M31" s="2" t="s">
-        <v>160</v>
+        <v>60</v>
       </c>
       <c r="N31" t="s">
-        <v>88</v>
+        <v>163</v>
       </c>
       <c r="O31" t="s">
-        <v>8</v>
+        <v>169</v>
       </c>
       <c r="P31" s="2" t="s">
-        <v>161</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>6</v>
+        <v>98</v>
       </c>
       <c r="B32" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="C32" t="s">
         <v>3</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>162</v>
+        <v>62</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>155</v>
+        <v>56</v>
       </c>
       <c r="G32" t="s">
-        <v>71</v>
+        <v>128</v>
       </c>
       <c r="H32" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="I32" t="s">
-        <v>89</v>
+        <v>37</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>157</v>
+        <v>58</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>159</v>
+        <v>59</v>
       </c>
       <c r="M32" s="2" t="s">
-        <v>160</v>
+        <v>60</v>
       </c>
       <c r="N32" t="s">
-        <v>90</v>
+        <v>164</v>
       </c>
       <c r="O32" t="s">
-        <v>8</v>
+        <v>169</v>
       </c>
       <c r="P32" s="2" t="s">
-        <v>161</v>
+        <v>61</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>6</v>
+        <v>98</v>
       </c>
       <c r="B33" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C33" t="s">
         <v>3</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>162</v>
+        <v>62</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>155</v>
+        <v>56</v>
       </c>
       <c r="G33" t="s">
-        <v>29</v>
+        <v>129</v>
       </c>
       <c r="H33" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="I33" t="s">
-        <v>91</v>
+        <v>38</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>157</v>
+        <v>58</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>159</v>
+        <v>59</v>
       </c>
       <c r="M33" s="2" t="s">
-        <v>160</v>
+        <v>60</v>
       </c>
       <c r="N33" t="s">
-        <v>92</v>
+        <v>165</v>
       </c>
       <c r="O33" t="s">
-        <v>8</v>
+        <v>169</v>
       </c>
       <c r="P33" s="2" t="s">
-        <v>161</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>6</v>
+        <v>98</v>
       </c>
       <c r="B34" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C34" t="s">
         <v>3</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>162</v>
+        <v>62</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>155</v>
+        <v>56</v>
       </c>
       <c r="G34" t="s">
-        <v>95</v>
+        <v>130</v>
       </c>
       <c r="H34" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="I34" t="s">
-        <v>93</v>
+        <v>39</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>157</v>
+        <v>58</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>159</v>
+        <v>59</v>
       </c>
       <c r="M34" s="2" t="s">
-        <v>160</v>
+        <v>60</v>
       </c>
       <c r="N34" t="s">
-        <v>94</v>
+        <v>166</v>
       </c>
       <c r="O34" t="s">
-        <v>8</v>
+        <v>169</v>
       </c>
       <c r="P34" s="2" t="s">
-        <v>161</v>
+        <v>61</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>33</v>
+        <v>98</v>
       </c>
       <c r="B35" t="s">
         <v>96</v>
@@ -3053,699 +3074,205 @@
         <v>3</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>162</v>
+        <v>62</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>155</v>
+        <v>56</v>
       </c>
       <c r="G35" t="s">
-        <v>98</v>
+        <v>131</v>
       </c>
       <c r="H35" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="I35" t="s">
-        <v>96</v>
+        <v>40</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>157</v>
+        <v>58</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>159</v>
+        <v>59</v>
       </c>
       <c r="M35" s="2" t="s">
-        <v>160</v>
+        <v>60</v>
       </c>
       <c r="N35" t="s">
-        <v>97</v>
+        <v>167</v>
       </c>
       <c r="O35" t="s">
-        <v>8</v>
+        <v>169</v>
       </c>
       <c r="P35" s="2" t="s">
-        <v>161</v>
+        <v>61</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>33</v>
+        <v>98</v>
       </c>
       <c r="B36" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C36" t="s">
         <v>3</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>162</v>
+        <v>62</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>155</v>
+        <v>56</v>
       </c>
       <c r="G36" t="s">
-        <v>101</v>
+        <v>132</v>
       </c>
       <c r="H36" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="I36" t="s">
-        <v>99</v>
+        <v>41</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>157</v>
+        <v>58</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="L36" s="2" t="s">
-        <v>159</v>
+        <v>59</v>
       </c>
       <c r="M36" s="2" t="s">
-        <v>160</v>
+        <v>60</v>
       </c>
       <c r="N36" t="s">
-        <v>100</v>
+        <v>168</v>
       </c>
       <c r="O36" t="s">
-        <v>8</v>
+        <v>169</v>
       </c>
       <c r="P36" s="2" t="s">
-        <v>161</v>
+        <v>61</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>33</v>
-      </c>
-      <c r="B37" t="s">
-        <v>102</v>
-      </c>
-      <c r="C37" t="s">
-        <v>3</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="G37" t="s">
-        <v>104</v>
-      </c>
-      <c r="H37" t="s">
-        <v>7</v>
-      </c>
-      <c r="I37" t="s">
-        <v>102</v>
-      </c>
-      <c r="J37" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="K37" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="L37" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="M37" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="N37" t="s">
-        <v>103</v>
-      </c>
-      <c r="O37" t="s">
-        <v>8</v>
-      </c>
-      <c r="P37" s="2" t="s">
-        <v>161</v>
-      </c>
+      <c r="D37" s="3"/>
+      <c r="E37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+      <c r="P37" s="2"/>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>33</v>
-      </c>
-      <c r="B38" t="s">
-        <v>105</v>
-      </c>
-      <c r="C38" t="s">
-        <v>3</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="G38" t="s">
-        <v>107</v>
-      </c>
-      <c r="H38" t="s">
-        <v>7</v>
-      </c>
-      <c r="I38" t="s">
-        <v>105</v>
-      </c>
-      <c r="J38" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="K38" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="L38" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="M38" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="N38" t="s">
-        <v>106</v>
-      </c>
-      <c r="O38" t="s">
-        <v>8</v>
-      </c>
-      <c r="P38" s="2" t="s">
-        <v>161</v>
-      </c>
+      <c r="D38" s="3"/>
+      <c r="E38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
+      <c r="P38" s="2"/>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>33</v>
-      </c>
-      <c r="B39" t="s">
-        <v>108</v>
-      </c>
-      <c r="C39" t="s">
-        <v>3</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="G39" t="s">
-        <v>110</v>
-      </c>
-      <c r="H39" t="s">
-        <v>7</v>
-      </c>
-      <c r="I39" t="s">
-        <v>108</v>
-      </c>
-      <c r="J39" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="K39" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="L39" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="M39" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="N39" t="s">
-        <v>109</v>
-      </c>
-      <c r="O39" t="s">
-        <v>8</v>
-      </c>
-      <c r="P39" s="2" t="s">
-        <v>161</v>
-      </c>
+      <c r="D39" s="3"/>
+      <c r="E39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
+      <c r="M39" s="2"/>
+      <c r="P39" s="2"/>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>33</v>
-      </c>
-      <c r="B40" t="s">
-        <v>111</v>
-      </c>
-      <c r="C40" t="s">
-        <v>3</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="G40" t="s">
-        <v>113</v>
-      </c>
-      <c r="H40" t="s">
-        <v>7</v>
-      </c>
-      <c r="I40" t="s">
-        <v>111</v>
-      </c>
-      <c r="J40" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="K40" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="L40" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="M40" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="N40" t="s">
-        <v>112</v>
-      </c>
-      <c r="O40" t="s">
-        <v>8</v>
-      </c>
-      <c r="P40" s="2" t="s">
-        <v>161</v>
-      </c>
+      <c r="D40" s="3"/>
+      <c r="E40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+      <c r="P40" s="2"/>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>33</v>
-      </c>
-      <c r="B41" t="s">
-        <v>114</v>
-      </c>
-      <c r="C41" t="s">
-        <v>3</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="G41" t="s">
-        <v>116</v>
-      </c>
-      <c r="H41" t="s">
-        <v>7</v>
-      </c>
-      <c r="I41" t="s">
-        <v>114</v>
-      </c>
-      <c r="J41" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="K41" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="L41" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="M41" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="N41" t="s">
-        <v>115</v>
-      </c>
-      <c r="O41" t="s">
-        <v>8</v>
-      </c>
-      <c r="P41" s="2" t="s">
-        <v>161</v>
-      </c>
+      <c r="D41" s="3"/>
+      <c r="E41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+      <c r="P41" s="2"/>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>33</v>
-      </c>
-      <c r="B42" t="s">
-        <v>117</v>
-      </c>
-      <c r="C42" t="s">
-        <v>3</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="G42" t="s">
-        <v>119</v>
-      </c>
-      <c r="H42" t="s">
-        <v>7</v>
-      </c>
-      <c r="I42" t="s">
-        <v>117</v>
-      </c>
-      <c r="J42" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="K42" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="L42" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="M42" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="N42" t="s">
-        <v>118</v>
-      </c>
-      <c r="O42" t="s">
-        <v>8</v>
-      </c>
-      <c r="P42" s="2" t="s">
-        <v>161</v>
-      </c>
+      <c r="D42" s="3"/>
+      <c r="E42" s="2"/>
+      <c r="J42" s="2"/>
+      <c r="K42" s="2"/>
+      <c r="L42" s="2"/>
+      <c r="M42" s="2"/>
+      <c r="P42" s="2"/>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>33</v>
-      </c>
-      <c r="B43" t="s">
-        <v>120</v>
-      </c>
-      <c r="C43" t="s">
-        <v>3</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="G43" t="s">
-        <v>122</v>
-      </c>
-      <c r="H43" t="s">
-        <v>7</v>
-      </c>
-      <c r="I43" t="s">
-        <v>120</v>
-      </c>
-      <c r="J43" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="K43" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="L43" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="M43" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="N43" t="s">
-        <v>121</v>
-      </c>
-      <c r="O43" t="s">
-        <v>8</v>
-      </c>
-      <c r="P43" s="2" t="s">
-        <v>161</v>
-      </c>
+      <c r="D43" s="3"/>
+      <c r="E43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+      <c r="L43" s="2"/>
+      <c r="M43" s="2"/>
+      <c r="P43" s="2"/>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>33</v>
-      </c>
-      <c r="B44" t="s">
-        <v>123</v>
-      </c>
-      <c r="C44" t="s">
-        <v>3</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="G44" t="s">
-        <v>125</v>
-      </c>
-      <c r="H44" t="s">
-        <v>7</v>
-      </c>
-      <c r="I44" t="s">
-        <v>123</v>
-      </c>
-      <c r="J44" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="K44" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="L44" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="M44" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="N44" t="s">
-        <v>124</v>
-      </c>
-      <c r="O44" t="s">
-        <v>8</v>
-      </c>
-      <c r="P44" s="2" t="s">
-        <v>161</v>
-      </c>
+      <c r="D44" s="3"/>
+      <c r="E44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
+      <c r="M44" s="2"/>
+      <c r="P44" s="2"/>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>33</v>
-      </c>
-      <c r="B45" t="s">
-        <v>126</v>
-      </c>
-      <c r="C45" t="s">
-        <v>3</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="G45" t="s">
-        <v>128</v>
-      </c>
-      <c r="H45" t="s">
-        <v>7</v>
-      </c>
-      <c r="I45" t="s">
-        <v>126</v>
-      </c>
-      <c r="J45" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="K45" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="L45" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="M45" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="N45" t="s">
-        <v>127</v>
-      </c>
-      <c r="O45" t="s">
-        <v>8</v>
-      </c>
-      <c r="P45" s="2" t="s">
-        <v>161</v>
-      </c>
+      <c r="D45" s="3"/>
+      <c r="E45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+      <c r="L45" s="2"/>
+      <c r="M45" s="2"/>
+      <c r="P45" s="2"/>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>33</v>
-      </c>
-      <c r="B46" t="s">
-        <v>129</v>
-      </c>
-      <c r="C46" t="s">
-        <v>3</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="G46" t="s">
-        <v>131</v>
-      </c>
-      <c r="H46" t="s">
-        <v>7</v>
-      </c>
-      <c r="I46" t="s">
-        <v>129</v>
-      </c>
-      <c r="J46" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="K46" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="L46" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="M46" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="N46" t="s">
-        <v>130</v>
-      </c>
-      <c r="O46" t="s">
-        <v>8</v>
-      </c>
-      <c r="P46" s="2" t="s">
-        <v>161</v>
-      </c>
+      <c r="D46" s="3"/>
+      <c r="E46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+      <c r="L46" s="2"/>
+      <c r="M46" s="2"/>
+      <c r="P46" s="2"/>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>33</v>
-      </c>
-      <c r="B47" t="s">
-        <v>132</v>
-      </c>
-      <c r="C47" t="s">
-        <v>3</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="G47" t="s">
-        <v>134</v>
-      </c>
-      <c r="H47" t="s">
-        <v>7</v>
-      </c>
-      <c r="I47" t="s">
-        <v>132</v>
-      </c>
-      <c r="J47" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="K47" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="L47" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="M47" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="N47" t="s">
-        <v>133</v>
-      </c>
-      <c r="O47" t="s">
-        <v>8</v>
-      </c>
-      <c r="P47" s="2" t="s">
-        <v>161</v>
-      </c>
+      <c r="D47" s="3"/>
+      <c r="E47" s="2"/>
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
+      <c r="L47" s="2"/>
+      <c r="M47" s="2"/>
+      <c r="P47" s="2"/>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>33</v>
-      </c>
-      <c r="B48" t="s">
-        <v>135</v>
-      </c>
-      <c r="C48" t="s">
-        <v>3</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="G48" t="s">
-        <v>137</v>
-      </c>
-      <c r="H48" t="s">
-        <v>7</v>
-      </c>
-      <c r="I48" t="s">
-        <v>135</v>
-      </c>
-      <c r="J48" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="K48" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="L48" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="M48" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="N48" t="s">
-        <v>136</v>
-      </c>
-      <c r="O48" t="s">
-        <v>8</v>
-      </c>
-      <c r="P48" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>33</v>
-      </c>
-      <c r="B49" t="s">
-        <v>138</v>
-      </c>
-      <c r="C49" t="s">
-        <v>3</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="G49" t="s">
-        <v>140</v>
-      </c>
-      <c r="H49" t="s">
-        <v>7</v>
-      </c>
-      <c r="I49" t="s">
-        <v>138</v>
-      </c>
-      <c r="J49" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="K49" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="L49" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="M49" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="N49" t="s">
-        <v>139</v>
-      </c>
-      <c r="O49" t="s">
-        <v>8</v>
-      </c>
-      <c r="P49" s="2" t="s">
-        <v>161</v>
-      </c>
+      <c r="D48" s="3"/>
+      <c r="E48" s="2"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="2"/>
+      <c r="L48" s="2"/>
+      <c r="M48" s="2"/>
+      <c r="P48" s="2"/>
+    </row>
+    <row r="49" spans="4:16" x14ac:dyDescent="0.25">
+      <c r="D49" s="3"/>
+      <c r="E49" s="2"/>
+      <c r="J49" s="2"/>
+      <c r="K49" s="2"/>
+      <c r="L49" s="2"/>
+      <c r="M49" s="2"/>
+      <c r="P49" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="20" type="noConversion"/>

</xml_diff>